<commit_message>
Database Changed to FAISS, Logic Changed for agents
</commit_message>
<xml_diff>
--- a/helpline_log.xlsx
+++ b/helpline_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,14 +541,58 @@
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>9386776366</t>
-        </is>
+      <c r="D5" t="n">
+        <v>9386776366</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>issue where website is not working, my name is Nisu purohit and number is 9386776366</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-06-04T23:11:42.841563</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Abhinab Kuamr</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>89871BZ</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Trouble opening the portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-06-04T23:12:15.948330</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Manish Guota</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8724B</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>unable to open loan account. Name: Manish Guota, id : 8724B</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed query logging issure where query wasnt logged properly
</commit_message>
<xml_diff>
--- a/helpline_log.xlsx
+++ b/helpline_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Query</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -482,6 +487,7 @@
           <t>Unable to upload second tranche on the portal</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,6 +511,7 @@
           <t>Having trouble opening the portal</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -528,6 +535,7 @@
           <t>Unable to contact officials</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -549,6 +557,7 @@
           <t>issue where website is not working, my name is Nisu purohit and number is 9386776366</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -572,6 +581,7 @@
           <t>Trouble opening the portal</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -593,6 +603,277 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>unable to open loan account. Name: Manish Guota, id : 8724B</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-06-13T18:57:46.456198</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Abhinab Kumar</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Name: Abhinab Kumar, Mobile Number: 9386776366</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-06-13T18:59:17.712704</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Abhinab</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>8787878787</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Name: Abhinab, Mobile Number: 8787878787</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:00:44.873436</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Abhinab</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>unable to upload docs</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:01:08.962484</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Akash Kr</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Report an issue</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:02:56.754380</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Abhinab Kumare</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Please describe the issue you are facing.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:03:12.631977</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Abhinab Kumare</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Unable to upload docs</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:08:56.093580</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Abhinab Kumar</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Please also describe your issue.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:32:20.394277</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Nishant Kumar</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ABCZYX1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Unable to get money</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:41:24.522473</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Aditya Thakur</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Report an Issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:43:02.460239</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Aditya Thakue</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>9386776366</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>unable to do anything</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:46:53.270003</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Bittu Kumar</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>9892BX</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Unable to open docs</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-06-13T19:51:08.681914</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Abhinab Kumar</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>87654BX</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Unable to log in</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added District and added threshold to model
</commit_message>
<xml_diff>
--- a/helpline_log.xlsx
+++ b/helpline_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Issue</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -488,6 +493,7 @@
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -512,6 +518,7 @@
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -536,6 +543,7 @@
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -558,6 +566,7 @@
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -582,6 +591,7 @@
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -606,6 +616,7 @@
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -628,6 +639,7 @@
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -650,6 +662,7 @@
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -672,6 +685,7 @@
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -694,6 +708,7 @@
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -716,6 +731,7 @@
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -738,6 +754,7 @@
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -760,6 +777,7 @@
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -784,6 +802,7 @@
           <t>Unable to get money</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -806,6 +825,7 @@
           <t>Report an Issue</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -828,6 +848,7 @@
           <t>unable to do anything</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -852,6 +873,7 @@
           <t>Unable to open docs</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -874,6 +896,65 @@
       <c r="F19" t="inlineStr">
         <is>
           <t>Unable to log in</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-06-14T16:35:38.750325</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Abhinab Kumar</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>BX7891</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Unable to open portal</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Vaishali</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-06-15T01:01:05.355001</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Abinab kr</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>785669bx</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>muje 2nd tranche nhi mila hai</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Patna</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Language Library changed to lingua
</commit_message>
<xml_diff>
--- a/helpline_log.xlsx
+++ b/helpline_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -958,6 +958,64 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-06-16T18:03:53.816246</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Abhinab</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>8876BX</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>portal nhi khul rha</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Patna</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-06-16T20:27:06.038859</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ashu Prasad</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>IONCBX</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>unable to get payment</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Patna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Issue format for logging
</commit_message>
<xml_diff>
--- a/helpline_log.xlsx
+++ b/helpline_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1016,6 +1016,35 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-06-17T02:03:43.065517</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Akash</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>9386776355</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Unable to get second tranche</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Sonpur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>